<commit_message>
running all proposals including final agreement for summary figures and tables
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_FINAL_AGREEMENT.xlsx
+++ b/app/data/wto_proposal_settings_master_FINAL_AGREEMENT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A74A3B-AB68-9842-876E-20B3CEE1B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91302380-5C21-8F43-9536-7C9A33E0C5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="1140" windowWidth="34160" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="492">
   <si>
     <t>proposal</t>
   </si>
@@ -1417,73 +1417,85 @@
     <t>JUNE 2022 Chair's text</t>
   </si>
   <si>
+    <t>Chair's text - June 2022</t>
+  </si>
+  <si>
+    <t>Chair's text (June) - Final draft</t>
+  </si>
+  <si>
+    <t>Final agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most ambitous scenario considering only subsidy types that fall directly under the scope of the final agreement, excluding those subtypes that include port construction and infrastructure. </t>
+  </si>
+  <si>
+    <t>Most ambitious scenario - elimination of subsidies covered by the scope of the agreement</t>
+  </si>
+  <si>
+    <t>WT/MIN(22)/W/20</t>
+  </si>
+  <si>
+    <t>Second Draft agreement - MC12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This Chair's text considered Members' comments and views in all discussions based on the previous consolidated draft documents (TN/RL/W/276 and Revs. 1 &amp; 2). This new text aims to capture the progress that Members have made since WT/MIN(21)/W/5 was issued. This text also suggests compromises on outstanding issues, meaning that it contains some new langugage. This text is without predudice of the position of any Member in respect of any issue. </t>
+  </si>
+  <si>
+    <t>Ministerial Conference Decision</t>
+  </si>
+  <si>
+    <t>Ministerial Conference - Agreement on Fisheries Subsidies - Ministerial Decision - June 17, 2022</t>
+  </si>
+  <si>
+    <t>Final text of the agreement agreed by Trade Ministers at the 12 WTO Ministerial Conference</t>
+  </si>
+  <si>
+    <t>Subsidies granted by developing and LDC Members shall be allowed for fishing in their own EEZ. As written, this exemption would only apply for a transition period of 2 years, but for the purposes of modeling we assume it to apply indefinitely.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsidies granted by developing and LDC Members shall be allowed for fishing in their own EEZ. As written, this exemption would only apply for a transition period of 2 years, but for the purposes of mdeling we assume it to apply indefinitely. </t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. It is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could only be acquired by vessels fulfilling our management criteria. We note that this may still be a conservative interpretation of this text because our management criteria are determined based on the location in which the fishing takes place, as opposed to by the flag- or subsidizing Member state.&lt;/li&gt;&lt;li&gt;This text would also prohibit subsidies to fishing in areas beyond the subsidizing Member's national jurisdiction.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas or in the EEZs of other coastal states to be prohibited. We note that this may be an amibitious interpretation of the prohibition on subsidies to fishing in areas beyond national jurisdictions.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for low income, resource-poor, or livelihood fishing in their territorial seas. For the purposes of modeling, we provide this exemption for developing countries for all fishing in their territorial waters (Note: as written the text also includes as an alternative 24 nautical miles but this is not modeled) unless they are responsible for more than 10% of annual global marine capture production. Developing Members responsible for less than 0.8% of global marine capture production will also be allowed to continue providing subsidies for fishing in their EEZs and in the areas of competence of RFMO/As as per the most recent published FAO data. As written, developing Members not meeting this criteria may also be allowed to provide subsidies for fishing in their EEZs and in the areas of competence of RFMO/As for a transition period, but this is not modeled.</t>
+  </si>
+  <si>
+    <t>TER10/CAP08</t>
+  </si>
+  <si>
+    <t>Boat construction and modernization, Fisheries development projects, Non-fuel tax exemptions, Fishing access agreements, Fuel subsidies, Fisher assistance, Vessel buyback programs, Rural fisher communities</t>
+  </si>
+  <si>
+    <t>B1, B2, B5, B6, B7, C1, C2, C3</t>
+  </si>
+  <si>
+    <t>Most ambitious scenario - limited subsidy scope</t>
+  </si>
+  <si>
+    <t>Final Fisheries Subsidies Agreement [no HS prohibition]</t>
+  </si>
+  <si>
+    <t>Final WTO Fisheries Subsidies Agreement - can't model HS portion because it's difficult to determine "unregulated HS"</t>
+  </si>
+  <si>
+    <t>WT/MIN(22)/W/22 | No prohibition for HS fishing</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale wehther vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond Members' national jurisdictions. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited. We note that this may be an amibitious interpretation of this prohibition.&lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale wehther vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that subsidies to vessels fishing beyond Members' national jurisdictions are allowed. We note that this may be a conservative interpretation of this prohibition.&lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>Final Fisheries Subsidies Agreement</t>
+  </si>
+  <si>
+    <t>WT/MIN(22)/W/22</t>
+  </si>
+  <si>
     <t>Final WTO Fisheries Subsidies Agreement</t>
-  </si>
-  <si>
-    <t>Chair's text - June 2022</t>
-  </si>
-  <si>
-    <t>Chair's text (June) - Final draft</t>
-  </si>
-  <si>
-    <t>Final agreement</t>
-  </si>
-  <si>
-    <t>Final Fisheries Subsidies Agreement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most ambitous scenario considering only subsidy types that fall directly under the scope of the final agreement, excluding those subtypes that include port construction and infrastructure. </t>
-  </si>
-  <si>
-    <t>Most ambitious scenario - elimination of subsidies covered by the scope of the agreement</t>
-  </si>
-  <si>
-    <t>WT/MIN(22)/W/20</t>
-  </si>
-  <si>
-    <t>Second Draft agreement - MC12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This Chair's text considered Members' comments and views in all discussions based on the previous consolidated draft documents (TN/RL/W/276 and Revs. 1 &amp; 2). This new text aims to capture the progress that Members have made since WT/MIN(21)/W/5 was issued. This text also suggests compromises on outstanding issues, meaning that it contains some new langugage. This text is without predudice of the position of any Member in respect of any issue. </t>
-  </si>
-  <si>
-    <t>WT/MIN(22)/W/22</t>
-  </si>
-  <si>
-    <t>Ministerial Conference Decision</t>
-  </si>
-  <si>
-    <t>Ministerial Conference - Agreement on Fisheries Subsidies - Ministerial Decision - June 17, 2022</t>
-  </si>
-  <si>
-    <t>Final text of the agreement agreed by Trade Ministers at the 12 WTO Ministerial Conference</t>
-  </si>
-  <si>
-    <t>Subsidies granted by developing and LDC Members shall be allowed for fishing in their own EEZ. As written, this exemption would only apply for a transition period of 2 years, but for the purposes of modeling we assume it to apply indefinitely.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subsidies granted by developing and LDC Members shall be allowed for fishing in their own EEZ. As written, this exemption would only apply for a transition period of 2 years, but for the purposes of mdeling we assume it to apply indefinitely. </t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) unless a Member can demonstrate that measures are implemented to maintain stocks at a biologically sustainable level. It is unclear how many Members would be able to satisfy this sustainability criteria, and thus we assume that such an exemption could only be acquired by vessels fulfilling our management criteria. We note that this may still be a conservative interpretation of this text because our management criteria are determined based on the location in which the fishing takes place, as opposed to by the flag- or subsidizing Member state.&lt;/li&gt;&lt;li&gt;This text would also prohibit subsidies to fishing in areas beyond the subsidizing Member's national jurisdiction.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas or in the EEZs of other coastal states to be prohibited. We note that this may be an amibitious interpretation of the prohibition on subsidies to fishing in areas beyond national jurisdictions.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>Subsidies granted by LDCs shall be allowed, and subsidies granted by developing countries shall be allowed for low income, resource-poor, or livelihood fishing in their territorial seas. For the purposes of modeling, we provide this exemption for developing countries for all fishing in their territorial waters (Note: as written the text also includes as an alternative 24 nautical miles but this is not modeled) unless they are responsible for more than 10% of annual global marine capture production. Developing Members responsible for less than 0.8% of global marine capture production will also be allowed to continue providing subsidies for fishing in their EEZs and in the areas of competence of RFMO/As as per the most recent published FAO data. As written, developing Members not meeting this criteria may also be allowed to provide subsidies for fishing in their EEZs and in the areas of competence of RFMO/As for a transition period, but this is not modeled.</t>
-  </si>
-  <si>
-    <t>TER10/CAP08</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale wehther vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond that Member's national jurisdiction. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas or in the EEZs of other coastal states to be prohibited. We note that this may be an amibitious interpretation of this prohibition.&lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>Boat construction and modernization, Fisheries development projects, Non-fuel tax exemptions, Fishing access agreements, Fuel subsidies, Fisher assistance, Vessel buyback programs, Rural fisher communities</t>
-  </si>
-  <si>
-    <t>B1, B2, B5, B6, B7, C1, C2, C3</t>
-  </si>
-  <si>
-    <t>Most ambitious scenario - limited subsidy scope</t>
   </si>
 </sst>
 </file>
@@ -2447,11 +2459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CV54"/>
+  <dimension ref="A1:CV55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -8145,16 +8157,16 @@
         <v>464</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F51" s="9">
         <v>44722</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>39</v>
@@ -8163,28 +8175,28 @@
         <v>330</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L51" s="20" t="s">
         <v>453</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="N51" s="20" t="s">
         <v>446</v>
       </c>
       <c r="O51" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="P51" s="20" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="Q51" s="20" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="R51" s="20" t="s">
         <v>38</v>
@@ -8269,7 +8281,7 @@
         <v>157</v>
       </c>
       <c r="BR51" s="7" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="BU51" s="8" t="s">
         <v>150</v>
@@ -8286,46 +8298,46 @@
         <v>302</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>469</v>
+        <v>489</v>
       </c>
       <c r="F52" s="9">
         <v>44729</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>475</v>
+        <v>490</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L52" s="20" t="s">
         <v>453</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="N52" s="20" t="s">
         <v>446</v>
       </c>
       <c r="O52" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="P52" s="20" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="Q52" s="20" t="s">
         <v>236</v>
@@ -8394,7 +8406,7 @@
         <v>181</v>
       </c>
       <c r="BF52" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BH52" s="8">
         <v>5</v>
@@ -8408,51 +8420,119 @@
     </row>
     <row r="53" spans="1:100" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>39</v>
+        <v>463</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>302</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="D53" s="10"/>
+        <v>485</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>467</v>
+      </c>
       <c r="E53" s="10" t="s">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="F53" s="9">
-        <v>44775</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>487</v>
-      </c>
-      <c r="H53" s="7" t="s">
+        <v>44729</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>486</v>
+      </c>
+      <c r="H53" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="I53" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>475</v>
+      </c>
       <c r="L53" s="20" t="s">
-        <v>238</v>
+        <v>453</v>
+      </c>
+      <c r="M53" s="20" t="s">
+        <v>476</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>238</v>
+        <v>446</v>
+      </c>
+      <c r="O53" s="20" t="s">
+        <v>477</v>
       </c>
       <c r="P53" s="20" t="s">
-        <v>485</v>
+        <v>488</v>
+      </c>
+      <c r="Q53" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="R53" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="S53" s="8" t="s">
+        <v>282</v>
       </c>
       <c r="T53" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="V53" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="Y53" s="8" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="Z53" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA53" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC53" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD53" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF53" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI53" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="AJ53" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AN53" s="8">
+        <v>5</v>
       </c>
       <c r="AQ53" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BD53" s="8" t="s">
-        <v>486</v>
+        <v>157</v>
+      </c>
+      <c r="AR53" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS53" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV53" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AW53" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AZ53" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="BE53" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="BH53" s="8">
+        <v>5</v>
+      </c>
       <c r="BL53" s="8" t="s">
         <v>150</v>
       </c>
@@ -8460,212 +8540,266 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:100" ht="42" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:100" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="F54" s="9">
+        <v>44775</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="H54" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="G54" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>39</v>
+      <c r="L54" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="N54" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="P54" s="20" t="s">
+        <v>481</v>
       </c>
       <c r="T54" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="U54" s="8">
-        <v>20</v>
-      </c>
-      <c r="V54" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="Y54" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="Z54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AC54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AF54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AJ54" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="AM54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AN54" s="8">
-        <v>24</v>
-      </c>
-      <c r="AO54" s="8">
-        <v>100</v>
-      </c>
-      <c r="AP54" s="8">
-        <v>400</v>
-      </c>
       <c r="AQ54" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="AR54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AU54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AV54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="AX54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AY54" s="8">
-        <v>5</v>
-      </c>
-      <c r="AZ54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BB54" s="8">
-        <v>5</v>
-      </c>
-      <c r="BC54" s="8">
-        <v>5</v>
+      <c r="BD54" s="8" t="s">
+        <v>482</v>
       </c>
       <c r="BE54" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="BH54" s="8">
+      <c r="BL54" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BY54" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:100" ht="42" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="G55" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="U55" s="8">
+        <v>20</v>
+      </c>
+      <c r="V55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB55" s="8">
         <v>5</v>
       </c>
-      <c r="BI54" s="8">
+      <c r="AC55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE55" s="8">
+        <v>5</v>
+      </c>
+      <c r="AF55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH55" s="8">
+        <v>5</v>
+      </c>
+      <c r="AJ55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM55" s="8">
+        <v>5</v>
+      </c>
+      <c r="AN55" s="8">
         <v>24</v>
       </c>
-      <c r="BJ54" s="8">
+      <c r="AO55" s="8">
         <v>100</v>
       </c>
-      <c r="BK54" s="8">
+      <c r="AP55" s="8">
         <v>400</v>
       </c>
-      <c r="BL54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BM54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BO54" s="8">
+      <c r="AQ55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT55" s="8">
         <v>5</v>
       </c>
-      <c r="BP54" s="8">
+      <c r="AU55" s="8">
         <v>5</v>
       </c>
-      <c r="BQ54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BS54" s="8">
+      <c r="AV55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AX55" s="8">
         <v>5</v>
       </c>
-      <c r="BT54" s="8">
+      <c r="AY55" s="8">
         <v>5</v>
       </c>
-      <c r="BU54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BW54" s="8">
+      <c r="AZ55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BB55" s="8">
         <v>5</v>
       </c>
-      <c r="BX54" s="8">
+      <c r="BC55" s="8">
         <v>5</v>
       </c>
-      <c r="BY54" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="BZ54" s="8" t="s">
+      <c r="BE55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="BH55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BI55" s="8">
+        <v>24</v>
+      </c>
+      <c r="BJ55" s="8">
+        <v>100</v>
+      </c>
+      <c r="BK55" s="8">
+        <v>400</v>
+      </c>
+      <c r="BL55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BM55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BP55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BQ55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BT55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BU55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BW55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BX55" s="8">
+        <v>5</v>
+      </c>
+      <c r="BY55" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="BZ55" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="CA54" s="8" t="s">
+      <c r="CA55" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="CB54" s="8" t="s">
+      <c r="CB55" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="CC54" s="8">
+      <c r="CC55" s="8">
         <v>0.7</v>
       </c>
-      <c r="CD54" s="8" t="s">
+      <c r="CD55" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="CE54" s="8" t="s">
+      <c r="CE55" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="CF54" s="8">
+      <c r="CF55" s="8">
         <v>50</v>
       </c>
-      <c r="CG54" s="14">
+      <c r="CG55" s="14">
         <v>5</v>
       </c>
-      <c r="CH54" s="14">
+      <c r="CH55" s="14">
         <v>5</v>
       </c>
-      <c r="CI54" s="14">
+      <c r="CI55" s="14">
         <v>5</v>
       </c>
-      <c r="CJ54" s="14">
+      <c r="CJ55" s="14">
         <v>5</v>
       </c>
-      <c r="CK54" s="8" t="s">
+      <c r="CK55" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="CL54" s="8">
+      <c r="CL55" s="8">
         <v>5</v>
       </c>
-      <c r="CM54" s="8">
+      <c r="CM55" s="8">
         <v>5</v>
       </c>
-      <c r="CN54" s="14">
+      <c r="CN55" s="14">
         <v>5</v>
       </c>
-      <c r="CO54" s="14">
+      <c r="CO55" s="14">
         <v>5</v>
       </c>
-      <c r="CP54" s="14">
+      <c r="CP55" s="14">
         <v>5</v>
       </c>
-      <c r="CQ54" s="8" t="s">
+      <c r="CQ55" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="CR54" s="8">
+      <c r="CR55" s="8">
         <v>5</v>
       </c>
-      <c r="CS54" s="8">
+      <c r="CS55" s="8">
         <v>5</v>
       </c>
-      <c r="CT54" s="14">
+      <c r="CT55" s="14">
         <v>5</v>
       </c>
-      <c r="CU54" s="14">
+      <c r="CU55" s="14">
         <v>5</v>
       </c>
-      <c r="CV54" s="14">
+      <c r="CV55" s="14">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
third option for final agreement
</commit_message>
<xml_diff>
--- a/app/data/wto_proposal_settings_master_FINAL_AGREEMENT.xlsx
+++ b/app/data/wto_proposal_settings_master_FINAL_AGREEMENT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kat/Github/SubsidyExplorer/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37109A7-3070-E44B-A447-96FD4A463A1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B1CB18-5503-394B-880B-3BDD65C0477B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61600" yWindow="-2480" windowWidth="23760" windowHeight="27200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35180" yWindow="-2480" windowWidth="50180" windowHeight="27200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="487">
   <si>
     <t>proposal</t>
   </si>
@@ -1432,15 +1432,6 @@
     <t>WT/MIN(22)/W/22 | No prohibition for HS fishing</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale wehther vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond Members' national jurisdictions. By default, we consider all capacity-enhancing subsidies provided to vessels spending at least 5% of their total annual effort fishing on the high seas to be prohibited. We note that this may be an amibitious interpretation of this prohibition.&lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>Final Fisheries Subsidies Agreement</t>
-  </si>
-  <si>
-    <t>WT/MIN(22)/W/22</t>
-  </si>
-  <si>
     <t>Final WTO Fisheries Subsidies Agreement</t>
   </si>
   <si>
@@ -1466,6 +1457,30 @@
   </si>
   <si>
     <t>TER/CAPTURE</t>
+  </si>
+  <si>
+    <t>Final Fisheries Subsidies Agreement [complete HS prohibition]</t>
+  </si>
+  <si>
+    <t>Final WTO Fisheries Subsidies Agreement - HS portion only applies to vessels that are not longline or purse seine</t>
+  </si>
+  <si>
+    <t>Final Fisheries Subsidies Agreement [non-tuna HS prohibition]</t>
+  </si>
+  <si>
+    <t>WT/MIN(22)/W/22 | Complete prohibition for HS fishing</t>
+  </si>
+  <si>
+    <t>WT/MIN(22)/W/22 | Non-tuna prohibition for HS fishing</t>
+  </si>
+  <si>
+    <t>HS/TUNA</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale wehther vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to vessels fishing in areas beyond Members' national jurisdictions. By default, we consider vessels spending at least 5% of their total annual effort fishing on the high seas to be affected. We note that this may be an amibitious interpretation of this prohibition.&lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;As written, this text would prohibit all capacity-enhancing and ambiguous subsidies as defined by Sumaila et al. (2019) to fishing in areas beyond the subsidizing Member's national jurisdiction and outside the competence of regional fisheries management organizations or agreements (RFMO/As).&lt;/li&gt;&lt;li&gt;Very few areas of the ocean are not under the jurisdiction of a RFMO/A, but it is difficult to determine on a global scale whether vessels are fishing for species governed by those RFMO/As at any given point in time.&lt;/li&gt;&lt;li&gt;We therefore assume that all capacity-enhancing an ambiguous subsidies as defined by Sumaila et al. (2019) are prohibited to non-tuna vessels fishing in areas beyond Members' national jurisdictions. We assume vessels utilizing the following gear types to be tuna fishing vessels: purse seines, drifting longlines, and pole and line. By default, we consider non-tuna fishing vessels spending at least 5% of their total annual effort fishing on the high seas to be affected. &lt;/li&gt;&lt;li&gt;For the purposes of modeling, the rules on reflagging and unassessed stocks are not considered.&lt;/ol&gt;</t>
   </si>
 </sst>
 </file>
@@ -2417,11 +2432,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN55"/>
+  <dimension ref="A1:CN56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BM60" sqref="BM60"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2553,10 +2568,10 @@
         <v>12</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="AL1" s="3" t="s">
         <v>13</v>
@@ -2604,10 +2619,10 @@
         <v>18</v>
       </c>
       <c r="BA1" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="BB1" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="BC1" s="3" t="s">
         <v>19</v>
@@ -2640,7 +2655,7 @@
         <v>132</v>
       </c>
       <c r="BM1" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="BN1" s="3" t="s">
         <v>133</v>
@@ -7636,7 +7651,7 @@
         <v>144</v>
       </c>
       <c r="BL47" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="BM47" s="6">
         <v>0.7</v>
@@ -7913,7 +7928,7 @@
         <v>144</v>
       </c>
       <c r="BL49" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="BM49" s="6">
         <v>0.7</v>
@@ -8059,7 +8074,7 @@
         <v>144</v>
       </c>
       <c r="BL50" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="BM50" s="6">
         <v>0.7</v>
@@ -8103,7 +8118,7 @@
         <v>456</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="L51" s="17" t="s">
         <v>438</v>
@@ -8159,9 +8174,6 @@
       <c r="AG51" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="AM51" s="6">
-        <v>5</v>
-      </c>
       <c r="AP51" s="6" t="s">
         <v>144</v>
       </c>
@@ -8205,7 +8217,7 @@
         <v>144</v>
       </c>
       <c r="BL51" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="BM51" s="6">
         <v>0.8</v>
@@ -8225,19 +8237,19 @@
         <v>289</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>452</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="F52" s="7">
         <v>44729</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>39</v>
@@ -8264,7 +8276,7 @@
         <v>461</v>
       </c>
       <c r="P52" s="17" t="s">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="Q52" s="17" t="s">
         <v>223</v>
@@ -8304,9 +8316,6 @@
       </c>
       <c r="AG52" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="AM52" s="6">
-        <v>5</v>
       </c>
       <c r="AP52" s="6" t="s">
         <v>144</v>
@@ -8347,7 +8356,7 @@
     </row>
     <row r="53" spans="1:92" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>448</v>
+        <v>39</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>289</v>
@@ -8392,7 +8401,7 @@
         <v>461</v>
       </c>
       <c r="P53" s="17" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="Q53" s="17" t="s">
         <v>223</v>
@@ -8432,9 +8441,6 @@
       </c>
       <c r="AG53" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="AM53" s="6">
-        <v>5</v>
       </c>
       <c r="AP53" s="6" t="s">
         <v>144</v>
@@ -8469,50 +8475,121 @@
     </row>
     <row r="54" spans="1:92" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>448</v>
+        <v>39</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>289</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>453</v>
-      </c>
-      <c r="D54" s="8"/>
+        <v>480</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>452</v>
+      </c>
       <c r="E54" s="8" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="F54" s="7">
-        <v>44775</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>466</v>
+        <v>44729</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>483</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="I54" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>459</v>
+      </c>
       <c r="L54" s="17" t="s">
-        <v>225</v>
+        <v>438</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>460</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>225</v>
+        <v>431</v>
+      </c>
+      <c r="O54" s="17" t="s">
+        <v>461</v>
       </c>
       <c r="P54" s="17" t="s">
-        <v>464</v>
+        <v>486</v>
+      </c>
+      <c r="Q54" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="R54" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="T54" s="6" t="s">
         <v>137</v>
       </c>
+      <c r="V54" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="Y54" s="6" t="s">
-        <v>137</v>
+        <v>144</v>
+      </c>
+      <c r="Z54" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA54" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB54" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC54" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD54" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF54" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG54" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="AP54" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ54" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AR54" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS54" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AT54" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU54" s="6" t="s">
         <v>137</v>
       </c>
       <c r="AW54" s="6" t="s">
-        <v>465</v>
+        <v>177</v>
       </c>
       <c r="AX54" s="6" t="s">
-        <v>136</v>
+        <v>168</v>
+      </c>
+      <c r="AY54" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC54" s="6">
+        <v>5</v>
       </c>
       <c r="BG54" s="6" t="s">
         <v>137</v>
@@ -8521,176 +8598,230 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:92" ht="42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:92" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>448</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+        <v>289</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="F55" s="7">
+        <v>44775</v>
+      </c>
       <c r="G55" s="6" t="s">
-        <v>51</v>
+        <v>466</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="L55" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="P55" s="17" t="s">
+        <v>464</v>
+      </c>
       <c r="T55" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="U55" s="6">
+      <c r="Y55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW55" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="AX55" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="BG55" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BQ55" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:92" ht="42" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="G56" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U56" s="6">
         <v>20</v>
       </c>
-      <c r="V55" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AG55" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL55" s="6">
+      <c r="V56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL56" s="6">
         <v>5</v>
       </c>
-      <c r="AM55" s="6">
+      <c r="AM56" s="6">
         <v>24</v>
       </c>
-      <c r="AN55" s="6">
+      <c r="AN56" s="6">
         <v>100</v>
       </c>
-      <c r="AO55" s="6">
+      <c r="AO56" s="6">
         <v>400</v>
       </c>
-      <c r="AP55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AQ55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AS55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AU55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AX55" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="BC55" s="6">
+      <c r="AP56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC56" s="6">
         <v>5</v>
       </c>
-      <c r="BD55" s="6">
+      <c r="BD56" s="6">
         <v>24</v>
       </c>
-      <c r="BE55" s="6">
+      <c r="BE56" s="6">
         <v>100</v>
       </c>
-      <c r="BF55" s="6">
+      <c r="BF56" s="6">
         <v>400</v>
       </c>
-      <c r="BG55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BH55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BJ55" s="6">
+      <c r="BG56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BJ56" s="6">
         <v>5</v>
       </c>
-      <c r="BK55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BM55" s="6">
+      <c r="BK56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BM56" s="6">
         <v>0.7</v>
       </c>
-      <c r="BN55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BP55" s="6">
+      <c r="BN56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BP56" s="6">
         <v>5</v>
       </c>
-      <c r="BQ55" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="BR55" s="6" t="s">
+      <c r="BQ56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BR56" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="BS55" s="6" t="s">
+      <c r="BS56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="BT55" s="6" t="s">
+      <c r="BT56" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="BU55" s="6">
+      <c r="BU56" s="6">
         <v>0.7</v>
       </c>
-      <c r="BV55" s="6" t="s">
+      <c r="BV56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="BW55" s="6" t="s">
+      <c r="BW56" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="BX55" s="6">
+      <c r="BX56" s="6">
         <v>50</v>
       </c>
-      <c r="BY55" s="6">
+      <c r="BY56" s="6">
         <v>5</v>
       </c>
-      <c r="BZ55" s="6">
+      <c r="BZ56" s="6">
         <v>5</v>
       </c>
-      <c r="CA55" s="6">
+      <c r="CA56" s="6">
         <v>5</v>
       </c>
-      <c r="CB55" s="6">
+      <c r="CB56" s="6">
         <v>5</v>
       </c>
-      <c r="CC55" s="6" t="s">
+      <c r="CC56" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="CD55" s="6">
+      <c r="CD56" s="6">
         <v>5</v>
       </c>
-      <c r="CE55" s="6">
+      <c r="CE56" s="6">
         <v>5</v>
       </c>
-      <c r="CF55" s="6">
+      <c r="CF56" s="6">
         <v>5</v>
       </c>
-      <c r="CG55" s="6">
+      <c r="CG56" s="6">
         <v>5</v>
       </c>
-      <c r="CH55" s="6">
+      <c r="CH56" s="6">
         <v>5</v>
       </c>
-      <c r="CI55" s="6" t="s">
+      <c r="CI56" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="CJ55" s="6">
+      <c r="CJ56" s="6">
         <v>5</v>
       </c>
-      <c r="CK55" s="6">
+      <c r="CK56" s="6">
         <v>5</v>
       </c>
-      <c r="CL55" s="6">
+      <c r="CL56" s="6">
         <v>5</v>
       </c>
-      <c r="CM55" s="6">
+      <c r="CM56" s="6">
         <v>5</v>
       </c>
-      <c r="CN55" s="6">
+      <c r="CN56" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>